<commit_message>
Version mejorada minimamente de carpeta de Tecnologia. Version mejorando todos los CashFlows para Negocio. Todavia falta SLA en las factibilidades.
</commit_message>
<xml_diff>
--- a/Gomez Marcos - Escenario de Perdida - contingencia.xlsx
+++ b/Gomez Marcos - Escenario de Perdida - contingencia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" tabRatio="714" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" tabRatio="714" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mercado Meta" sheetId="4" r:id="rId1"/>
@@ -1732,6 +1732,14 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1840,17 +1848,6 @@
     <xf numFmtId="0" fontId="21" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1858,6 +1855,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2091,7 +2091,7 @@
                   <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>470</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,8 +2111,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="42870272"/>
-        <c:axId val="59836672"/>
+        <c:axId val="132299776"/>
+        <c:axId val="107144320"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2257,13 +2257,13 @@
                 <c:formatCode>[$$-2C0A]\ #,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1440000</c:v>
+                  <c:v>2160000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2880000</c:v>
+                  <c:v>4320000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5640000</c:v>
+                  <c:v>8640000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2285,11 +2285,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42880512"/>
-        <c:axId val="59837248"/>
+        <c:axId val="132497408"/>
+        <c:axId val="107144896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42870272"/>
+        <c:axId val="132299776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2332,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59836672"/>
+        <c:crossAx val="107144320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2340,7 +2340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59836672"/>
+        <c:axId val="107144320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,12 +2391,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42870272"/>
+        <c:crossAx val="132299776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59837248"/>
+        <c:axId val="107144896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2433,12 +2433,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42880512"/>
+        <c:crossAx val="132497408"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="42880512"/>
+        <c:axId val="132497408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2447,7 +2447,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59837248"/>
+        <c:crossAx val="107144896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2828,11 +2828,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45082112"/>
-        <c:axId val="59839552"/>
+        <c:axId val="132499456"/>
+        <c:axId val="107147200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45082112"/>
+        <c:axId val="132499456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2891,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59839552"/>
+        <c:crossAx val="107147200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2899,7 +2899,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59839552"/>
+        <c:axId val="107147200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2958,7 +2958,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45082112"/>
+        <c:crossAx val="132499456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3406,11 +3406,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45083136"/>
-        <c:axId val="59841856"/>
+        <c:axId val="59315712"/>
+        <c:axId val="107149504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45083136"/>
+        <c:axId val="59315712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3469,7 +3469,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59841856"/>
+        <c:crossAx val="107149504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3477,7 +3477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59841856"/>
+        <c:axId val="107149504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3536,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45083136"/>
+        <c:crossAx val="59315712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3804,40 +3804,40 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>37.6</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.900000000000006</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.2</c:v>
+                  <c:v>28.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.3</c:v>
+                  <c:v>43.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.6</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.25</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.900000000000006</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.6</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.6</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.3</c:v>
+                  <c:v>43.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.7</c:v>
+                  <c:v>52.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.050000000000004</c:v>
+                  <c:v>55.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3984,11 +3984,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45083648"/>
-        <c:axId val="45631168"/>
+        <c:axId val="132251648"/>
+        <c:axId val="133440064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45083648"/>
+        <c:axId val="132251648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4047,7 +4047,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45631168"/>
+        <c:crossAx val="133440064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4055,7 +4055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45631168"/>
+        <c:axId val="133440064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4114,7 +4114,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45083648"/>
+        <c:crossAx val="132251648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4783,64 +4783,64 @@
                 <c:formatCode>[$$-2C0A]\ #,##0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>12000</c:v>
+                  <c:v>18000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24000</c:v>
+                  <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36000</c:v>
+                  <c:v>54000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48000</c:v>
+                  <c:v>72000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60000</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72000</c:v>
+                  <c:v>108000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84000</c:v>
+                  <c:v>126000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>96000</c:v>
+                  <c:v>144000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>108000</c:v>
+                  <c:v>162000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>120000</c:v>
+                  <c:v>180000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>132000</c:v>
+                  <c:v>198000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>144000</c:v>
+                  <c:v>216000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>156000</c:v>
+                  <c:v>234000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>168000</c:v>
+                  <c:v>252000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>180000</c:v>
+                  <c:v>270000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>192000</c:v>
+                  <c:v>288000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>204000</c:v>
+                  <c:v>306000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>216000</c:v>
+                  <c:v>324000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>228000</c:v>
+                  <c:v>342000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>240000</c:v>
+                  <c:v>360000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4862,11 +4862,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45080576"/>
-        <c:axId val="45633472"/>
+        <c:axId val="132252160"/>
+        <c:axId val="133442368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45080576"/>
+        <c:axId val="132252160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4930,7 +4930,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45633472"/>
+        <c:crossAx val="133442368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4938,7 +4938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45633472"/>
+        <c:axId val="133442368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4997,7 +4997,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45080576"/>
+        <c:crossAx val="132252160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8789,7 +8789,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8800,7 +8800,7 @@
   <dimension ref="A3:E16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A4" sqref="A4:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8837,7 +8837,7 @@
         <v>240</v>
       </c>
       <c r="D5" s="24">
-        <v>470</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8846,15 +8846,15 @@
       </c>
       <c r="B6" s="75">
         <f>E16*B5</f>
-        <v>1440000</v>
+        <v>2160000</v>
       </c>
       <c r="C6" s="75">
         <f>E16*C5</f>
-        <v>2880000</v>
+        <v>4320000</v>
       </c>
       <c r="D6" s="75">
         <f>E16*D5</f>
-        <v>5640000</v>
+        <v>8640000</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
@@ -8880,7 +8880,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" s="15">
-        <v>12000</v>
+        <v>18000</v>
       </c>
     </row>
   </sheetData>
@@ -8910,16 +8910,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="175" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="173"/>
-      <c r="E1" s="171" t="s">
+      <c r="B1" s="176"/>
+      <c r="C1" s="177"/>
+      <c r="E1" s="175" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="172"/>
-      <c r="G1" s="173"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="177"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9114,16 +9114,16 @@
       <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="175" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="172"/>
-      <c r="C13" s="173"/>
-      <c r="E13" s="171" t="s">
+      <c r="B13" s="176"/>
+      <c r="C13" s="177"/>
+      <c r="E13" s="175" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="172"/>
-      <c r="G13" s="173"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="177"/>
       <c r="H13" s="49" t="s">
         <v>144</v>
       </c>
@@ -9313,16 +9313,16 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="171" t="s">
+      <c r="A25" s="175" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="173"/>
-      <c r="E25" s="171" t="s">
+      <c r="B25" s="176"/>
+      <c r="C25" s="177"/>
+      <c r="E25" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="F25" s="172"/>
-      <c r="G25" s="173"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="177"/>
       <c r="H25" s="49" t="s">
         <v>145</v>
       </c>
@@ -9348,7 +9348,7 @@
       </c>
       <c r="H26" s="50">
         <f>('Mercado Meta'!D5-'Mercado Meta'!C5)/'Mercado Meta'!C5</f>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -9369,7 +9369,7 @@
       </c>
       <c r="G27" s="9">
         <f>G31*H3</f>
-        <v>39166.666666666664</v>
+        <v>40000</v>
       </c>
       <c r="I27" s="44"/>
     </row>
@@ -9391,7 +9391,7 @@
       </c>
       <c r="G28" s="9">
         <f>G31*H4</f>
-        <v>5875</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -9412,7 +9412,7 @@
       </c>
       <c r="G29" s="9">
         <f>G31*H5</f>
-        <v>7050</v>
+        <v>7200</v>
       </c>
       <c r="H29" s="46"/>
       <c r="I29" s="30"/>
@@ -9456,7 +9456,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="13">
         <f>(G19*H26)+G19</f>
-        <v>122591.66666666667</v>
+        <v>125200</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="G32" s="13">
         <f>G31*12</f>
-        <v>1471100</v>
+        <v>1502400</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9529,7 +9529,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9549,18 +9549,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="174" t="s">
+      <c r="C1" s="178" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="175"/>
-      <c r="E1" s="174" t="s">
+      <c r="D1" s="179"/>
+      <c r="E1" s="178" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="175"/>
-      <c r="G1" s="174" t="s">
+      <c r="F1" s="179"/>
+      <c r="G1" s="178" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="175"/>
+      <c r="H1" s="179"/>
       <c r="I1" s="78"/>
       <c r="K1" s="137" t="s">
         <v>19</v>
@@ -9588,7 +9588,7 @@
       <c r="F2" s="80"/>
       <c r="G2" s="79">
         <f>'Mercado Meta'!D5/12</f>
-        <v>39.166666666666664</v>
+        <v>40</v>
       </c>
       <c r="H2" s="80"/>
       <c r="I2" s="81"/>
@@ -9605,7 +9605,7 @@
       </c>
       <c r="M2" s="80">
         <f>G2</f>
-        <v>39.166666666666664</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
@@ -9618,7 +9618,7 @@
       </c>
       <c r="D3" s="85">
         <f>C3*$L$11</f>
-        <v>120000</v>
+        <v>180000</v>
       </c>
       <c r="E3" s="84">
         <f>E2</f>
@@ -9626,15 +9626,15 @@
       </c>
       <c r="F3" s="85">
         <f>E3*$L$11</f>
-        <v>240000</v>
+        <v>360000</v>
       </c>
       <c r="G3" s="84">
         <f>G2</f>
-        <v>39.166666666666664</v>
+        <v>40</v>
       </c>
       <c r="H3" s="85">
         <f>G3*$L$11</f>
-        <v>470000</v>
+        <v>720000</v>
       </c>
       <c r="I3" s="86"/>
       <c r="J3" s="140" t="s">
@@ -9647,7 +9647,7 @@
       </c>
       <c r="M3" s="89">
         <f>(M2-L2)/L2</f>
-        <v>0.95833333333333326</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -9679,17 +9679,17 @@
       <c r="C5" s="94"/>
       <c r="D5" s="95">
         <f>D3+D4</f>
-        <v>120000</v>
+        <v>180000</v>
       </c>
       <c r="E5" s="93"/>
       <c r="F5" s="95">
         <f>F3+F4</f>
-        <v>240000</v>
+        <v>360000</v>
       </c>
       <c r="G5" s="93"/>
       <c r="H5" s="95">
         <f>H3+H4</f>
-        <v>470000</v>
+        <v>720000</v>
       </c>
       <c r="I5" s="96"/>
       <c r="J5" s="97"/>
@@ -9699,18 +9699,18 @@
     </row>
     <row r="6" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="176" t="s">
+      <c r="C7" s="180" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="177"/>
-      <c r="E7" s="176" t="s">
+      <c r="D7" s="181"/>
+      <c r="E7" s="180" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="177"/>
-      <c r="G7" s="176" t="s">
+      <c r="F7" s="181"/>
+      <c r="G7" s="180" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="177"/>
+      <c r="H7" s="181"/>
       <c r="I7" s="78"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -9729,7 +9729,7 @@
       <c r="F8" s="99"/>
       <c r="G8" s="100">
         <f>(E8*M3)+E8</f>
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="H8" s="99"/>
       <c r="I8" s="81"/>
@@ -9756,11 +9756,11 @@
       </c>
       <c r="G9" s="84">
         <f>G8</f>
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="H9" s="102">
         <f>G9*$M$4</f>
-        <v>5640000</v>
+        <v>5760000</v>
       </c>
       <c r="I9" s="86"/>
     </row>
@@ -9797,14 +9797,14 @@
       <c r="G11" s="93"/>
       <c r="H11" s="95">
         <f>H9+H10</f>
-        <v>5640000</v>
+        <v>5760000</v>
       </c>
       <c r="I11" s="96"/>
       <c r="K11" s="143" t="s">
         <v>172</v>
       </c>
       <c r="L11" s="15">
-        <v>12000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
@@ -9984,51 +9984,51 @@
       </c>
       <c r="C22" s="101">
         <f t="shared" ref="C22:N22" si="1">IFERROR(C21*$L$11,0)</f>
-        <v>14400</v>
+        <v>21600</v>
       </c>
       <c r="D22" s="101">
         <f t="shared" si="1"/>
-        <v>28800</v>
+        <v>43200</v>
       </c>
       <c r="E22" s="101">
         <f t="shared" si="1"/>
-        <v>57600</v>
+        <v>86400</v>
       </c>
       <c r="F22" s="101">
         <f t="shared" si="1"/>
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="G22" s="101">
         <f t="shared" si="1"/>
-        <v>115200</v>
+        <v>172800</v>
       </c>
       <c r="H22" s="101">
         <f t="shared" si="1"/>
-        <v>172799.99999999997</v>
+        <v>259199.99999999997</v>
       </c>
       <c r="I22" s="101">
         <f t="shared" si="1"/>
-        <v>144000</v>
+        <v>216000</v>
       </c>
       <c r="J22" s="101">
         <f t="shared" si="1"/>
-        <v>201600</v>
+        <v>302400</v>
       </c>
       <c r="K22" s="101">
         <f t="shared" si="1"/>
-        <v>187200.00000000003</v>
+        <v>280800</v>
       </c>
       <c r="L22" s="101">
         <f t="shared" si="1"/>
-        <v>230400</v>
+        <v>345600</v>
       </c>
       <c r="M22" s="101">
         <f t="shared" si="1"/>
-        <v>216000</v>
+        <v>324000</v>
       </c>
       <c r="N22" s="101">
         <f t="shared" si="1"/>
-        <v>1440000.0000000002</v>
+        <v>2160000.0000000005</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -10236,55 +10236,55 @@
       </c>
       <c r="B33" s="101">
         <f t="shared" ref="B33:C33" si="3">IFERROR(B32*$L$11,0)</f>
-        <v>230400</v>
+        <v>345600</v>
       </c>
       <c r="C33" s="101">
         <f t="shared" si="3"/>
-        <v>259199.99999999997</v>
+        <v>388799.99999999994</v>
       </c>
       <c r="D33" s="101">
         <f t="shared" ref="D33" si="4">IFERROR(D32*$L$11,0)</f>
-        <v>172799.99999999997</v>
+        <v>259199.99999999997</v>
       </c>
       <c r="E33" s="101">
         <f t="shared" ref="E33" si="5">IFERROR(E32*$L$11,0)</f>
-        <v>201600</v>
+        <v>302400</v>
       </c>
       <c r="F33" s="101">
         <f t="shared" ref="F33" si="6">IFERROR(F32*$L$11,0)</f>
-        <v>172799.99999999997</v>
+        <v>259199.99999999997</v>
       </c>
       <c r="G33" s="101">
         <f t="shared" ref="G33" si="7">IFERROR(G32*$L$11,0)</f>
-        <v>201600</v>
+        <v>302400</v>
       </c>
       <c r="H33" s="101">
         <f t="shared" ref="H33" si="8">IFERROR(H32*$L$11,0)</f>
-        <v>172799.99999999997</v>
+        <v>259199.99999999997</v>
       </c>
       <c r="I33" s="101">
         <f t="shared" ref="I33" si="9">IFERROR(I32*$L$11,0)</f>
-        <v>259199.99999999997</v>
+        <v>388799.99999999994</v>
       </c>
       <c r="J33" s="101">
         <f t="shared" ref="J33" si="10">IFERROR(J32*$L$11,0)</f>
-        <v>230400</v>
+        <v>345600</v>
       </c>
       <c r="K33" s="101">
         <f t="shared" ref="K33" si="11">IFERROR(K32*$L$11,0)</f>
-        <v>288000</v>
+        <v>432000</v>
       </c>
       <c r="L33" s="101">
         <f t="shared" ref="L33" si="12">IFERROR(L32*$L$11,0)</f>
-        <v>345599.99999999994</v>
+        <v>518399.99999999994</v>
       </c>
       <c r="M33" s="101">
         <f t="shared" ref="M33" si="13">IFERROR(M32*$L$11,0)</f>
-        <v>345599.99999999994</v>
+        <v>518399.99999999994</v>
       </c>
       <c r="N33" s="101">
         <f t="shared" ref="N33" si="14">IFERROR(N32*$L$11,0)</f>
-        <v>2880000</v>
+        <v>4320000</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -10328,7 +10328,7 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B40" s="106">
         <f>G9</f>
-        <v>470</v>
+        <v>480</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -10435,55 +10435,55 @@
       </c>
       <c r="B44" s="105">
         <f>$B$40*B42</f>
-        <v>37.6</v>
+        <v>38.4</v>
       </c>
       <c r="C44" s="105">
         <f t="shared" ref="C44:M44" si="15">$B$40*C42</f>
-        <v>32.900000000000006</v>
+        <v>33.6</v>
       </c>
       <c r="D44" s="105">
         <f t="shared" si="15"/>
-        <v>28.2</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="E44" s="105">
         <f t="shared" si="15"/>
-        <v>42.3</v>
+        <v>43.199999999999996</v>
       </c>
       <c r="F44" s="105">
         <f t="shared" si="15"/>
-        <v>37.6</v>
+        <v>38.4</v>
       </c>
       <c r="G44" s="105">
         <f t="shared" si="15"/>
-        <v>35.25</v>
+        <v>36</v>
       </c>
       <c r="H44" s="105">
         <f t="shared" si="15"/>
-        <v>32.900000000000006</v>
+        <v>33.6</v>
       </c>
       <c r="I44" s="105">
         <f t="shared" si="15"/>
-        <v>37.6</v>
+        <v>38.4</v>
       </c>
       <c r="J44" s="105">
         <f t="shared" si="15"/>
-        <v>37.6</v>
+        <v>38.4</v>
       </c>
       <c r="K44" s="105">
         <f t="shared" si="15"/>
-        <v>42.3</v>
+        <v>43.199999999999996</v>
       </c>
       <c r="L44" s="105">
         <f t="shared" si="15"/>
-        <v>51.7</v>
+        <v>52.8</v>
       </c>
       <c r="M44" s="105">
         <f t="shared" si="15"/>
-        <v>54.050000000000004</v>
+        <v>55.2</v>
       </c>
       <c r="N44" s="105">
         <f>SUM(B44:M44)</f>
-        <v>470.00000000000006</v>
+        <v>479.99999999999994</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -10492,55 +10492,55 @@
       </c>
       <c r="B45" s="101">
         <f t="shared" ref="B45:N45" si="16">IFERROR(B44*$L$11,0)</f>
-        <v>451200</v>
+        <v>691200</v>
       </c>
       <c r="C45" s="101">
         <f t="shared" si="16"/>
-        <v>394800.00000000006</v>
+        <v>604800</v>
       </c>
       <c r="D45" s="101">
         <f t="shared" si="16"/>
-        <v>338400</v>
+        <v>518399.99999999994</v>
       </c>
       <c r="E45" s="101">
         <f t="shared" si="16"/>
-        <v>507599.99999999994</v>
+        <v>777599.99999999988</v>
       </c>
       <c r="F45" s="101">
         <f t="shared" si="16"/>
-        <v>451200</v>
+        <v>691200</v>
       </c>
       <c r="G45" s="101">
         <f t="shared" si="16"/>
-        <v>423000</v>
+        <v>648000</v>
       </c>
       <c r="H45" s="101">
         <f t="shared" si="16"/>
-        <v>394800.00000000006</v>
+        <v>604800</v>
       </c>
       <c r="I45" s="101">
         <f t="shared" si="16"/>
-        <v>451200</v>
+        <v>691200</v>
       </c>
       <c r="J45" s="101">
         <f t="shared" si="16"/>
-        <v>451200</v>
+        <v>691200</v>
       </c>
       <c r="K45" s="101">
         <f t="shared" si="16"/>
-        <v>507599.99999999994</v>
+        <v>777599.99999999988</v>
       </c>
       <c r="L45" s="101">
         <f t="shared" si="16"/>
-        <v>620400</v>
+        <v>950400</v>
       </c>
       <c r="M45" s="101">
         <f t="shared" si="16"/>
-        <v>648600</v>
+        <v>993600</v>
       </c>
       <c r="N45" s="101">
         <f t="shared" si="16"/>
-        <v>5640000.0000000009</v>
+        <v>8639999.9999999981</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
@@ -10601,7 +10601,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10621,7 +10621,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="188" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -10635,7 +10635,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="185"/>
+      <c r="B4" s="189"/>
       <c r="C4" s="123" t="s">
         <v>10</v>
       </c>
@@ -10648,7 +10648,7 @@
       <c r="K4" s="30"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="185"/>
+      <c r="B5" s="189"/>
       <c r="C5" s="123" t="s">
         <v>13</v>
       </c>
@@ -10661,7 +10661,7 @@
       <c r="K5" s="109"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="185"/>
+      <c r="B6" s="189"/>
       <c r="C6" s="123" t="s">
         <v>11</v>
       </c>
@@ -10673,7 +10673,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="185"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="123" t="s">
         <v>5</v>
       </c>
@@ -10687,7 +10687,7 @@
       <c r="L7" s="113"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="185"/>
+      <c r="B8" s="189"/>
       <c r="C8" s="123" t="s">
         <v>6</v>
       </c>
@@ -10701,11 +10701,11 @@
         <v>173</v>
       </c>
       <c r="H8" s="37">
-        <v>12000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="185"/>
+      <c r="B9" s="189"/>
       <c r="C9" s="123" t="s">
         <v>7</v>
       </c>
@@ -10717,7 +10717,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="186"/>
+      <c r="B10" s="190"/>
       <c r="C10" s="126" t="s">
         <v>8</v>
       </c>
@@ -10729,7 +10729,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="184" t="s">
+      <c r="B11" s="188" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="123" t="s">
@@ -10743,7 +10743,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="185"/>
+      <c r="B12" s="189"/>
       <c r="C12" s="123" t="s">
         <v>15</v>
       </c>
@@ -10755,7 +10755,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="186"/>
+      <c r="B13" s="190"/>
       <c r="C13" s="129" t="s">
         <v>16</v>
       </c>
@@ -10767,10 +10767,10 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="187" t="s">
+      <c r="C14" s="191" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="188"/>
+      <c r="D14" s="192"/>
       <c r="E14" s="132">
         <f>SUM(E4:E13)</f>
         <v>159000</v>
@@ -10814,7 +10814,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="181" t="s">
+      <c r="A19" s="185" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="114">
@@ -10833,11 +10833,11 @@
       </c>
       <c r="F19" s="116">
         <f t="shared" ref="F19:F38" si="0">B19*$H$8</f>
-        <v>12000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="182"/>
+      <c r="A20" s="186"/>
       <c r="B20" s="114">
         <v>2</v>
       </c>
@@ -10855,11 +10855,11 @@
       </c>
       <c r="F20" s="116">
         <f t="shared" si="0"/>
-        <v>24000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="182"/>
+      <c r="A21" s="186"/>
       <c r="B21" s="114">
         <v>3</v>
       </c>
@@ -10877,11 +10877,11 @@
       </c>
       <c r="F21" s="116">
         <f t="shared" si="0"/>
-        <v>36000</v>
+        <v>54000</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="182"/>
+      <c r="A22" s="186"/>
       <c r="B22" s="114">
         <v>4</v>
       </c>
@@ -10899,11 +10899,11 @@
       </c>
       <c r="F22" s="116">
         <f t="shared" si="0"/>
-        <v>48000</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="182"/>
+      <c r="A23" s="186"/>
       <c r="B23" s="114">
         <v>5</v>
       </c>
@@ -10921,11 +10921,11 @@
       </c>
       <c r="F23" s="116">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="182"/>
+      <c r="A24" s="186"/>
       <c r="B24" s="114">
         <v>6</v>
       </c>
@@ -10943,11 +10943,11 @@
       </c>
       <c r="F24" s="116">
         <f t="shared" si="0"/>
-        <v>72000</v>
+        <v>108000</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="182"/>
+      <c r="A25" s="186"/>
       <c r="B25" s="114">
         <v>7</v>
       </c>
@@ -10965,11 +10965,11 @@
       </c>
       <c r="F25" s="116">
         <f t="shared" si="0"/>
-        <v>84000</v>
+        <v>126000</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="182"/>
+      <c r="A26" s="186"/>
       <c r="B26" s="114">
         <v>8</v>
       </c>
@@ -10987,11 +10987,11 @@
       </c>
       <c r="F26" s="116">
         <f t="shared" si="0"/>
-        <v>96000</v>
+        <v>144000</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="182"/>
+      <c r="A27" s="186"/>
       <c r="B27" s="114">
         <v>9</v>
       </c>
@@ -11009,11 +11009,11 @@
       </c>
       <c r="F27" s="116">
         <f t="shared" si="0"/>
-        <v>108000</v>
+        <v>162000</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="182"/>
+      <c r="A28" s="186"/>
       <c r="B28" s="114">
         <v>10</v>
       </c>
@@ -11031,11 +11031,11 @@
       </c>
       <c r="F28" s="116">
         <f t="shared" si="0"/>
-        <v>120000</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="182"/>
+      <c r="A29" s="186"/>
       <c r="B29" s="114">
         <v>11</v>
       </c>
@@ -11053,11 +11053,11 @@
       </c>
       <c r="F29" s="116">
         <f t="shared" si="0"/>
-        <v>132000</v>
+        <v>198000</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="182"/>
+      <c r="A30" s="186"/>
       <c r="B30" s="117">
         <v>12</v>
       </c>
@@ -11075,11 +11075,11 @@
       </c>
       <c r="F30" s="119">
         <f t="shared" si="0"/>
-        <v>144000</v>
+        <v>216000</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="182"/>
+      <c r="A31" s="186"/>
       <c r="B31" s="114">
         <v>13</v>
       </c>
@@ -11097,11 +11097,11 @@
       </c>
       <c r="F31" s="116">
         <f t="shared" si="0"/>
-        <v>156000</v>
+        <v>234000</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="183"/>
+      <c r="A32" s="187"/>
       <c r="B32" s="114">
         <v>14</v>
       </c>
@@ -11119,7 +11119,7 @@
       </c>
       <c r="F32" s="116">
         <f t="shared" si="0"/>
-        <v>168000</v>
+        <v>252000</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -11143,11 +11143,11 @@
       </c>
       <c r="F33" s="112">
         <f t="shared" si="0"/>
-        <v>180000</v>
+        <v>270000</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="178" t="s">
+      <c r="A34" s="182" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="120">
@@ -11167,11 +11167,11 @@
       </c>
       <c r="F34" s="122">
         <f t="shared" si="0"/>
-        <v>192000</v>
+        <v>288000</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="179"/>
+      <c r="A35" s="183"/>
       <c r="B35" s="120">
         <v>17</v>
       </c>
@@ -11189,11 +11189,11 @@
       </c>
       <c r="F35" s="122">
         <f t="shared" si="0"/>
-        <v>204000</v>
+        <v>306000</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="179"/>
+      <c r="A36" s="183"/>
       <c r="B36" s="120">
         <v>18</v>
       </c>
@@ -11211,11 +11211,11 @@
       </c>
       <c r="F36" s="122">
         <f t="shared" si="0"/>
-        <v>216000</v>
+        <v>324000</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="179"/>
+      <c r="A37" s="183"/>
       <c r="B37" s="120">
         <v>19</v>
       </c>
@@ -11233,11 +11233,11 @@
       </c>
       <c r="F37" s="122">
         <f t="shared" si="0"/>
-        <v>228000</v>
+        <v>342000</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="180"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="120">
         <v>20</v>
       </c>
@@ -11255,7 +11255,7 @@
       </c>
       <c r="F38" s="122">
         <f t="shared" si="0"/>
-        <v>240000</v>
+        <v>360000</v>
       </c>
     </row>
   </sheetData>
@@ -11276,8 +11276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11370,7 +11370,7 @@
       </c>
       <c r="J4" s="157">
         <f t="shared" si="0"/>
-        <v>360331.38749999995</v>
+        <v>391376.38749999995</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -11390,7 +11390,7 @@
       </c>
       <c r="E5" s="58">
         <f>Mensual!H11</f>
-        <v>5640000</v>
+        <v>5760000</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -11409,7 +11409,7 @@
       </c>
       <c r="E6" s="59">
         <f>Mensual!H11</f>
-        <v>5640000</v>
+        <v>5760000</v>
       </c>
       <c r="H6" s="55"/>
     </row>
@@ -11439,7 +11439,7 @@
       </c>
       <c r="E8" s="62">
         <f>-Costos!G32</f>
-        <v>-1471100</v>
+        <v>-1502400</v>
       </c>
       <c r="G8" s="153"/>
       <c r="H8" s="158" t="s">
@@ -11512,7 +11512,7 @@
       </c>
       <c r="J10" s="157">
         <f t="shared" si="1"/>
-        <v>169200</v>
+        <v>172800</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -11531,7 +11531,7 @@
       </c>
       <c r="E11" s="64">
         <f>SUM(E8:E10)</f>
-        <v>-4610481.75</v>
+        <v>-4641781.75</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -11559,7 +11559,7 @@
       </c>
       <c r="E13" s="66">
         <f>+E6+E11</f>
-        <v>1029518.25</v>
+        <v>1118218.25</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -11584,7 +11584,7 @@
       </c>
       <c r="E15" s="67">
         <f>-E13*0.35</f>
-        <v>-360331.38749999995</v>
+        <v>-391376.38749999995</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -11609,7 +11609,7 @@
       </c>
       <c r="E17" s="68">
         <f>E15+E13</f>
-        <v>669186.86250000005</v>
+        <v>726841.86250000005</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -11655,7 +11655,7 @@
       </c>
       <c r="E20" s="68">
         <f>SUM(E17:E19)</f>
-        <v>814808.61250000005</v>
+        <v>872463.61250000005</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -11682,7 +11682,7 @@
       </c>
       <c r="B23" s="168">
         <f>NPV(B22,C20,D20,E20)+B20</f>
-        <v>-410692.88652290357</v>
+        <v>-376349.79254528892</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -11691,7 +11691,7 @@
       </c>
       <c r="B24" s="169">
         <f>IRR(B20:E20,30)</f>
-        <v>-5.580573141207168E-2</v>
+        <v>-3.1135962394597705E-2</v>
       </c>
       <c r="G24" s="29"/>
     </row>
@@ -11748,19 +11748,19 @@
       <c r="G4" s="148" t="s">
         <v>139</v>
       </c>
-      <c r="H4" s="190" t="s">
+      <c r="H4" s="194" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="191"/>
-      <c r="J4" s="192"/>
+      <c r="I4" s="195"/>
+      <c r="J4" s="196"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="147" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="193"/>
-      <c r="C5" s="194"/>
-      <c r="D5" s="195"/>
+      <c r="B5" s="197"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="199"/>
       <c r="F5" s="147" t="s">
         <v>140</v>
       </c>
@@ -11913,18 +11913,18 @@
       <c r="A10" s="149" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="196"/>
-      <c r="C10" s="197"/>
-      <c r="D10" s="198"/>
+      <c r="B10" s="200"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="202"/>
       <c r="F10" s="149" t="s">
         <v>141</v>
       </c>
       <c r="G10" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="H10" s="199"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="201"/>
+      <c r="H10" s="203"/>
+      <c r="I10" s="204"/>
+      <c r="J10" s="205"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -11996,18 +11996,18 @@
       <c r="A13" s="149" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="196"/>
-      <c r="C13" s="197"/>
-      <c r="D13" s="198"/>
+      <c r="B13" s="200"/>
+      <c r="C13" s="201"/>
+      <c r="D13" s="202"/>
       <c r="F13" s="149" t="s">
         <v>112</v>
       </c>
       <c r="G13" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="H13" s="199"/>
-      <c r="I13" s="200"/>
-      <c r="J13" s="201"/>
+      <c r="H13" s="203"/>
+      <c r="I13" s="204"/>
+      <c r="J13" s="205"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
@@ -12112,18 +12112,18 @@
       <c r="A17" s="149" t="s">
         <v>142</v>
       </c>
-      <c r="B17" s="196"/>
-      <c r="C17" s="197"/>
-      <c r="D17" s="198"/>
+      <c r="B17" s="200"/>
+      <c r="C17" s="201"/>
+      <c r="D17" s="202"/>
       <c r="F17" s="149" t="s">
         <v>142</v>
       </c>
       <c r="G17" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="H17" s="199"/>
-      <c r="I17" s="200"/>
-      <c r="J17" s="201"/>
+      <c r="H17" s="203"/>
+      <c r="I17" s="204"/>
+      <c r="J17" s="205"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
@@ -12160,11 +12160,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="189" t="s">
+      <c r="A19" s="193" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="189"/>
-      <c r="C19" s="189"/>
+      <c r="B19" s="193"/>
+      <c r="C19" s="193"/>
       <c r="D19" s="43">
         <f>SUM(D6:D18)</f>
         <v>578134</v>
@@ -12199,17 +12199,17 @@
       <c r="A24" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="208" t="s">
+      <c r="B24" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="209" t="s">
+      <c r="C24" s="172" t="s">
         <v>178</v>
       </c>
-      <c r="D24" s="209"/>
-      <c r="E24" s="209" t="s">
+      <c r="D24" s="172"/>
+      <c r="E24" s="172" t="s">
         <v>182</v>
       </c>
-      <c r="F24" s="209" t="s">
+      <c r="F24" s="172" t="s">
         <v>179</v>
       </c>
     </row>
@@ -12217,7 +12217,7 @@
       <c r="A25" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="210">
+      <c r="B25" s="173">
         <f>D6</f>
         <v>36000</v>
       </c>
@@ -12237,7 +12237,7 @@
       <c r="A26" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="210">
+      <c r="B26" s="173">
         <f>D7</f>
         <v>30000</v>
       </c>
@@ -12257,7 +12257,7 @@
       <c r="A27" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="210">
+      <c r="B27" s="173">
         <f>D8</f>
         <v>16000</v>
       </c>
@@ -12277,7 +12277,7 @@
       <c r="A28" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="210">
+      <c r="B28" s="173">
         <f>D9</f>
         <v>45000</v>
       </c>
@@ -12303,7 +12303,7 @@
       <c r="A30" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="210">
+      <c r="B30" s="173">
         <f>D11</f>
         <v>150000</v>
       </c>
@@ -12323,7 +12323,7 @@
       <c r="A31" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="210">
+      <c r="B31" s="173">
         <f>D12</f>
         <v>5000</v>
       </c>
@@ -12340,10 +12340,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="209" t="s">
+      <c r="E32" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="211">
+      <c r="F32" s="174">
         <f>SUM(F25:F31)</f>
         <v>88900</v>
       </c>
@@ -12661,13 +12661,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="206" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="202"/>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="202"/>
+      <c r="B15" s="206"/>
+      <c r="C15" s="206"/>
+      <c r="D15" s="206"/>
+      <c r="E15" s="206"/>
       <c r="F15" s="151">
         <f>SUM(F4:F14)</f>
         <v>209475</v>
@@ -12686,7 +12686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -12741,20 +12741,20 @@
       </c>
       <c r="B5" s="145"/>
       <c r="C5" s="145"/>
-      <c r="D5" s="203" t="s">
+      <c r="D5" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="E5" s="203"/>
-      <c r="F5" s="203"/>
-      <c r="G5" s="203"/>
-      <c r="H5" s="203"/>
-      <c r="I5" s="203"/>
-      <c r="J5" s="203"/>
-      <c r="K5" s="203"/>
-      <c r="L5" s="203"/>
-      <c r="M5" s="203"/>
-      <c r="N5" s="203"/>
-      <c r="O5" s="203"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="207"/>
+      <c r="G5" s="207"/>
+      <c r="H5" s="207"/>
+      <c r="I5" s="207"/>
+      <c r="J5" s="207"/>
+      <c r="K5" s="207"/>
+      <c r="L5" s="207"/>
+      <c r="M5" s="207"/>
+      <c r="N5" s="207"/>
+      <c r="O5" s="207"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C6" s="76" t="s">
@@ -13047,20 +13047,20 @@
       </c>
       <c r="B15" s="145"/>
       <c r="C15" s="145"/>
-      <c r="D15" s="203" t="s">
+      <c r="D15" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="203"/>
-      <c r="F15" s="203"/>
-      <c r="G15" s="203"/>
-      <c r="H15" s="203"/>
-      <c r="I15" s="203"/>
-      <c r="J15" s="203"/>
-      <c r="K15" s="203"/>
-      <c r="L15" s="203"/>
-      <c r="M15" s="203"/>
-      <c r="N15" s="203"/>
-      <c r="O15" s="203"/>
+      <c r="E15" s="207"/>
+      <c r="F15" s="207"/>
+      <c r="G15" s="207"/>
+      <c r="H15" s="207"/>
+      <c r="I15" s="207"/>
+      <c r="J15" s="207"/>
+      <c r="K15" s="207"/>
+      <c r="L15" s="207"/>
+      <c r="M15" s="207"/>
+      <c r="N15" s="207"/>
+      <c r="O15" s="207"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="145"/>
@@ -13355,20 +13355,20 @@
       </c>
       <c r="B24" s="145"/>
       <c r="C24" s="145"/>
-      <c r="D24" s="203" t="s">
+      <c r="D24" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="203"/>
-      <c r="F24" s="203"/>
-      <c r="G24" s="203"/>
-      <c r="H24" s="203"/>
-      <c r="I24" s="203"/>
-      <c r="J24" s="203"/>
-      <c r="K24" s="203"/>
-      <c r="L24" s="203"/>
-      <c r="M24" s="203"/>
-      <c r="N24" s="203"/>
-      <c r="O24" s="203"/>
+      <c r="E24" s="207"/>
+      <c r="F24" s="207"/>
+      <c r="G24" s="207"/>
+      <c r="H24" s="207"/>
+      <c r="I24" s="207"/>
+      <c r="J24" s="207"/>
+      <c r="K24" s="207"/>
+      <c r="L24" s="207"/>
+      <c r="M24" s="207"/>
+      <c r="N24" s="207"/>
+      <c r="O24" s="207"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="145"/>
@@ -13680,20 +13680,20 @@
       </c>
       <c r="B33" s="145"/>
       <c r="C33" s="145"/>
-      <c r="D33" s="212" t="s">
+      <c r="D33" s="211" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="213"/>
-      <c r="F33" s="213"/>
-      <c r="G33" s="213"/>
-      <c r="H33" s="213"/>
-      <c r="I33" s="213"/>
-      <c r="J33" s="213"/>
-      <c r="K33" s="213"/>
-      <c r="L33" s="213"/>
-      <c r="M33" s="213"/>
-      <c r="N33" s="213"/>
-      <c r="O33" s="214"/>
+      <c r="E33" s="212"/>
+      <c r="F33" s="212"/>
+      <c r="G33" s="212"/>
+      <c r="H33" s="212"/>
+      <c r="I33" s="212"/>
+      <c r="J33" s="212"/>
+      <c r="K33" s="212"/>
+      <c r="L33" s="212"/>
+      <c r="M33" s="212"/>
+      <c r="N33" s="212"/>
+      <c r="O33" s="213"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C34" s="76" t="s">
@@ -14022,20 +14022,20 @@
       </c>
       <c r="B44" s="145"/>
       <c r="C44" s="145"/>
-      <c r="D44" s="212" t="s">
+      <c r="D44" s="211" t="s">
         <v>151</v>
       </c>
-      <c r="E44" s="213"/>
-      <c r="F44" s="213"/>
-      <c r="G44" s="213"/>
-      <c r="H44" s="213"/>
-      <c r="I44" s="213"/>
-      <c r="J44" s="213"/>
-      <c r="K44" s="213"/>
-      <c r="L44" s="213"/>
-      <c r="M44" s="213"/>
-      <c r="N44" s="213"/>
-      <c r="O44" s="214"/>
+      <c r="E44" s="212"/>
+      <c r="F44" s="212"/>
+      <c r="G44" s="212"/>
+      <c r="H44" s="212"/>
+      <c r="I44" s="212"/>
+      <c r="J44" s="212"/>
+      <c r="K44" s="212"/>
+      <c r="L44" s="212"/>
+      <c r="M44" s="212"/>
+      <c r="N44" s="212"/>
+      <c r="O44" s="213"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C45" s="76" t="s">
@@ -14328,20 +14328,20 @@
       </c>
       <c r="B54" s="145"/>
       <c r="C54" s="145"/>
-      <c r="D54" s="203" t="s">
+      <c r="D54" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="E54" s="203"/>
-      <c r="F54" s="203"/>
-      <c r="G54" s="203"/>
-      <c r="H54" s="203"/>
-      <c r="I54" s="203"/>
-      <c r="J54" s="203"/>
-      <c r="K54" s="203"/>
-      <c r="L54" s="203"/>
-      <c r="M54" s="203"/>
-      <c r="N54" s="203"/>
-      <c r="O54" s="203"/>
+      <c r="E54" s="207"/>
+      <c r="F54" s="207"/>
+      <c r="G54" s="207"/>
+      <c r="H54" s="207"/>
+      <c r="I54" s="207"/>
+      <c r="J54" s="207"/>
+      <c r="K54" s="207"/>
+      <c r="L54" s="207"/>
+      <c r="M54" s="207"/>
+      <c r="N54" s="207"/>
+      <c r="O54" s="207"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="145"/>
@@ -14634,20 +14634,20 @@
       <c r="A64" s="77" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="207" t="s">
+      <c r="D64" s="214" t="s">
         <v>151</v>
       </c>
-      <c r="E64" s="207"/>
-      <c r="F64" s="207"/>
-      <c r="G64" s="207"/>
-      <c r="H64" s="207"/>
-      <c r="I64" s="207"/>
-      <c r="J64" s="207"/>
-      <c r="K64" s="207"/>
-      <c r="L64" s="207"/>
-      <c r="M64" s="207"/>
-      <c r="N64" s="207"/>
-      <c r="O64" s="207"/>
+      <c r="E64" s="214"/>
+      <c r="F64" s="214"/>
+      <c r="G64" s="214"/>
+      <c r="H64" s="214"/>
+      <c r="I64" s="214"/>
+      <c r="J64" s="214"/>
+      <c r="K64" s="214"/>
+      <c r="L64" s="214"/>
+      <c r="M64" s="214"/>
+      <c r="N64" s="214"/>
+      <c r="O64" s="214"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C65" s="76" t="s">
@@ -14959,20 +14959,20 @@
       </c>
       <c r="B76" s="145"/>
       <c r="C76" s="145"/>
-      <c r="D76" s="203" t="s">
+      <c r="D76" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="E76" s="203"/>
-      <c r="F76" s="203"/>
-      <c r="G76" s="203"/>
-      <c r="H76" s="203"/>
-      <c r="I76" s="203"/>
-      <c r="J76" s="203"/>
-      <c r="K76" s="203"/>
-      <c r="L76" s="203"/>
-      <c r="M76" s="203"/>
-      <c r="N76" s="203"/>
-      <c r="O76" s="203"/>
+      <c r="E76" s="207"/>
+      <c r="F76" s="207"/>
+      <c r="G76" s="207"/>
+      <c r="H76" s="207"/>
+      <c r="I76" s="207"/>
+      <c r="J76" s="207"/>
+      <c r="K76" s="207"/>
+      <c r="L76" s="207"/>
+      <c r="M76" s="207"/>
+      <c r="N76" s="207"/>
+      <c r="O76" s="207"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="145"/>
@@ -15267,20 +15267,20 @@
       </c>
       <c r="B86" s="145"/>
       <c r="C86" s="145"/>
-      <c r="D86" s="203" t="s">
+      <c r="D86" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="E86" s="203"/>
-      <c r="F86" s="203"/>
-      <c r="G86" s="203"/>
-      <c r="H86" s="203"/>
-      <c r="I86" s="203"/>
-      <c r="J86" s="203"/>
-      <c r="K86" s="203"/>
-      <c r="L86" s="203"/>
-      <c r="M86" s="203"/>
-      <c r="N86" s="203"/>
-      <c r="O86" s="203"/>
+      <c r="E86" s="207"/>
+      <c r="F86" s="207"/>
+      <c r="G86" s="207"/>
+      <c r="H86" s="207"/>
+      <c r="I86" s="207"/>
+      <c r="J86" s="207"/>
+      <c r="K86" s="207"/>
+      <c r="L86" s="207"/>
+      <c r="M86" s="207"/>
+      <c r="N86" s="207"/>
+      <c r="O86" s="207"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="145"/>
@@ -15582,7 +15582,7 @@
       </c>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C99" s="204" t="s">
+      <c r="C99" s="208" t="s">
         <v>155</v>
       </c>
       <c r="D99" s="92">
@@ -15599,13 +15599,13 @@
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C100" s="205"/>
+      <c r="C100" s="209"/>
       <c r="D100" s="87"/>
       <c r="E100" s="87"/>
       <c r="F100" s="87"/>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C101" s="205"/>
+      <c r="C101" s="209"/>
       <c r="D101" s="87" t="s">
         <v>4</v>
       </c>
@@ -15617,7 +15617,7 @@
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C102" s="206"/>
+      <c r="C102" s="210"/>
       <c r="D102" s="92">
         <f>D99/12</f>
         <v>130000</v>

</xml_diff>